<commit_message>
Updates till EX4 MFA in matrix form
</commit_message>
<xml_diff>
--- a/EX2_W3_EW-MFA/EUROSTAT_Dataset_DPO_2014_2016.xlsx
+++ b/EX2_W3_EW-MFA/EUROSTAT_Dataset_DPO_2014_2016.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20390"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pang\Desktop\Stuff\_HERUS\MFA course\_Datasets for MFA exercises\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barsanti.INTRANET\Desktop\PhD\3_CODEs\ENV-501_MEFA_exercises\EX2_W3_EW-MFA\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB5920EC-5EB6-432E-8D2A-5DE29E95E375}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9804"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="6810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
@@ -75,10 +76,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="172" formatCode="dd\.mm\.yy"/>
-    <numFmt numFmtId="173" formatCode="#,##0.000"/>
+    <numFmt numFmtId="164" formatCode="dd\.mm\.yy"/>
+    <numFmt numFmtId="165" formatCode="#,##0.000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -133,13 +134,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="172" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="173" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -419,26 +421,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.59765625" customWidth="1"/>
-    <col min="2" max="4" width="14.09765625" customWidth="1"/>
+    <col min="1" max="1" width="13.625" customWidth="1"/>
+    <col min="2" max="4" width="14.125" customWidth="1"/>
     <col min="5" max="7" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -446,7 +448,7 @@
         <v>43648.649687500001</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -454,7 +456,7 @@
         <v>43656.623181365736</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -462,7 +464,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -470,7 +472,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>6</v>
       </c>
@@ -493,30 +495,30 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G10" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>13</v>
       </c>
@@ -539,7 +541,7 @@
         <v>7.173</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>14</v>
       </c>
@@ -562,7 +564,7 @@
         <v>7.2089999999999996</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>15</v>
       </c>
@@ -585,10 +587,10 @@
         <v>7.9059999999999997</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
     </row>

</xml_diff>